<commit_message>
changes to rooms tests
Regression testing complete
</commit_message>
<xml_diff>
--- a/TestFiles/availableRooms/availableroomsindex.xlsx
+++ b/TestFiles/availableRooms/availableroomsindex.xlsx
@@ -27,9 +27,6 @@
     <t>Input is not accepted. Missing room size.</t>
   </si>
   <si>
-    <t>Input is not accepted. Missing space between room name and room number.</t>
-  </si>
-  <si>
     <t>Input not accepeted. Proper spacing not maintained.</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     </r>
   </si>
   <si>
-    <t>Input is not accepted. Missing room type.</t>
-  </si>
-  <si>
     <t>Input is not accepted. Missing room information.</t>
   </si>
   <si>
@@ -238,6 +232,12 @@
   </si>
   <si>
     <t>Duplicate room names on line one and two. Input is accepted.</t>
+  </si>
+  <si>
+    <t>Line one input is not accepted. Missing room type.</t>
+  </si>
+  <si>
+    <t>Line one input is not accepted. Missing space between room name and room number.</t>
   </si>
 </sst>
 </file>
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -653,63 +653,63 @@
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>2</v>
@@ -717,186 +717,186 @@
     </row>
     <row r="10" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>